<commit_message>
feature/mx-1714 wrap up odk (#294)
# Changes
- wrap up odk model v3 update

---------

Signed-off-by: erichesse <eric.hesse3@yahoo.de>
Co-authored-by: Nicolas Drebenstedt <drebenstedtn@rki.de>
Co-authored-by: Nicolas Drebenstedt <897972+cutoffthetop@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/assets/raw-data/odk/test_raw_data.xlsx
+++ b/assets/raw-data/odk/test_raw_data.xlsx
@@ -1,25 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20415"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HesseE\mex-extractors\assets\raw-data\odk\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C3FE562-DF89-492D-9406-07903741A8AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="survey"/>
-    <sheet r:id="rId2" sheetId="2" name="choices"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_Hlk82596326" localSheetId="0">survey!#REF!</definedName>
     <definedName name="_Hlk88063113" localSheetId="0">survey!#REF!</definedName>
   </definedNames>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="79">
   <si>
     <t>list_name</t>
   </si>
@@ -69,9 +75,6 @@
     <t>Ke nokutjiwa</t>
   </si>
   <si>
-    <t>Refused to answer</t>
-  </si>
-  <si>
     <t>Ma panḓa okuzira</t>
   </si>
   <si>
@@ -88,9 +91,6 @@
   </si>
   <si>
     <t>Omukazendu we, omurumendu we, otjiyambura tje</t>
-  </si>
-  <si>
-    <t>Son or daughter</t>
   </si>
   <si>
     <t>Omuatje we omuzandu poo omukazona</t>
@@ -271,8 +271,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="0"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -321,7 +320,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFff0000"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -335,22 +334,22 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffc599"/>
+        <fgColor rgb="FFFFC599"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffff00"/>
+        <fgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF46bdc6"/>
+        <fgColor rgb="FF46BDC6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFffffff"/>
+        <fgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -389,94 +388,93 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="5" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="4" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="7" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="7" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="5" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -487,10 +485,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
@@ -528,71 +526,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -620,7 +618,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -643,11 +641,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -656,13 +654,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -672,7 +670,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -681,7 +679,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -690,7 +688,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -698,10 +696,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -766,7 +764,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -774,42 +772,28 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="25" width="25.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="25" width="24.862142857142857" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="25" width="81.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="25" width="80.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="26" width="41.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="26" width="4.433571428571429" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="26" width="51.14785714285715" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="26" width="5.576428571428571" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="26" width="11.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="26" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="26" width="9.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="12" max="12" style="26" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="13" max="13" style="26" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="14" max="14" style="26" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="15" max="15" style="26" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="16" max="16" style="26" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="17" max="17" style="26" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="18" max="18" style="26" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="19" max="19" style="26" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="20" max="20" style="26" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="21" max="21" style="26" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="22" max="22" style="26" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="23" max="23" style="26" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="24" max="24" style="26" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="25" max="25" style="26" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="26" max="26" style="26" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="25" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="81.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.7109375" style="26" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="51.140625" style="26" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.5703125" style="26" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" style="26" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.85546875" style="26" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" style="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="26" width="14.140625" style="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="1" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C1" s="8" t="s">
         <v>1</v>
@@ -818,7 +802,7 @@
         <v>2</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F1" s="8"/>
       <c r="G1" s="9"/>
@@ -842,12 +826,12 @@
       <c r="Y1" s="8"/>
       <c r="Z1" s="8"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="2" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -874,18 +858,18 @@
       <c r="Y2" s="10"/>
       <c r="Z2" s="10"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="3" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
@@ -910,18 +894,18 @@
       <c r="Y3" s="12"/>
       <c r="Z3" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="4" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="D4" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="C4" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>34</v>
       </c>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
@@ -946,18 +930,18 @@
       <c r="Y4" s="12"/>
       <c r="Z4" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="5" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
@@ -982,18 +966,18 @@
       <c r="Y5" s="12"/>
       <c r="Z5" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="6" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E6" s="12"/>
       <c r="F6" s="12"/>
@@ -1018,18 +1002,18 @@
       <c r="Y6" s="12"/>
       <c r="Z6" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="7" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E7" s="12"/>
       <c r="F7" s="12"/>
@@ -1054,18 +1038,18 @@
       <c r="Y7" s="12"/>
       <c r="Z7" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="8" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>43</v>
-      </c>
       <c r="D8" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E8" s="12"/>
       <c r="F8" s="12"/>
@@ -1090,7 +1074,7 @@
       <c r="Y8" s="12"/>
       <c r="Z8" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="9" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="13"/>
       <c r="B9" s="13"/>
       <c r="C9" s="13"/>
@@ -1118,18 +1102,18 @@
       <c r="Y9" s="12"/>
       <c r="Z9" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="10" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>45</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" s="10" t="s">
-        <v>47</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="10"/>
@@ -1154,7 +1138,7 @@
       <c r="Y10" s="12"/>
       <c r="Z10" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="11" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="13"/>
       <c r="B11" s="13"/>
       <c r="C11" s="13"/>
@@ -1182,7 +1166,7 @@
       <c r="Y11" s="12"/>
       <c r="Z11" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="12" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="13"/>
       <c r="B12" s="13"/>
       <c r="C12" s="14"/>
@@ -1210,18 +1194,18 @@
       <c r="Y12" s="12"/>
       <c r="Z12" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="13" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="C13" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="D13" s="16" t="s">
         <v>49</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="D13" s="16" t="s">
-        <v>51</v>
       </c>
       <c r="E13" s="17"/>
       <c r="F13" s="10"/>
@@ -1246,18 +1230,18 @@
       <c r="Y13" s="12"/>
       <c r="Z13" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="14" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>54</v>
-      </c>
       <c r="D14" s="10" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E14" s="12"/>
       <c r="F14" s="10"/>
@@ -1282,21 +1266,21 @@
       <c r="Y14" s="12"/>
       <c r="Z14" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="15" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="E15" s="10" t="s">
         <v>57</v>
-      </c>
-      <c r="D15" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>59</v>
       </c>
       <c r="F15" s="12"/>
       <c r="G15" s="12"/>
@@ -1320,21 +1304,21 @@
       <c r="Y15" s="12"/>
       <c r="Z15" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="16" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="C16" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="10" t="s">
-        <v>62</v>
-      </c>
       <c r="E16" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F16" s="12"/>
       <c r="G16" s="12"/>
@@ -1358,18 +1342,18 @@
       <c r="Y16" s="12"/>
       <c r="Z16" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="17" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B17" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>63</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>65</v>
       </c>
       <c r="E17" s="12"/>
       <c r="F17" s="12"/>
@@ -1394,18 +1378,18 @@
       <c r="Y17" s="12"/>
       <c r="Z17" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="18" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B18" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="D18" s="10" t="s">
         <v>66</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="10" t="s">
-        <v>68</v>
       </c>
       <c r="E18" s="17"/>
       <c r="F18" s="10"/>
@@ -1430,18 +1414,18 @@
       <c r="Y18" s="12"/>
       <c r="Z18" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="19" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B19" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>69</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="D19" s="10" t="s">
-        <v>71</v>
       </c>
       <c r="E19" s="17"/>
       <c r="F19" s="10"/>
@@ -1466,15 +1450,15 @@
       <c r="Y19" s="12"/>
       <c r="Z19" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="20" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D20" s="10"/>
       <c r="E20" s="17"/>
@@ -1500,7 +1484,7 @@
       <c r="Y20" s="12"/>
       <c r="Z20" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="21" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="13"/>
       <c r="B21" s="13"/>
       <c r="C21" s="19"/>
@@ -1528,18 +1512,18 @@
       <c r="Y21" s="12"/>
       <c r="Z21" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="22" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B22" s="21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C22" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D22" s="21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E22" s="12"/>
       <c r="F22" s="12"/>
@@ -1564,18 +1548,18 @@
       <c r="Y22" s="12"/>
       <c r="Z22" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="23" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B23" s="22" t="s">
+        <v>73</v>
+      </c>
+      <c r="C23" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B23" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>46</v>
-      </c>
       <c r="D23" s="22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E23" s="12"/>
       <c r="F23" s="12"/>
@@ -1600,18 +1584,18 @@
       <c r="Y23" s="12"/>
       <c r="Z23" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="24" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="22" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B24" s="22" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E24" s="12"/>
       <c r="F24" s="12"/>
@@ -1636,18 +1620,18 @@
       <c r="Y24" s="12"/>
       <c r="Z24" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="25" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="22" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B25" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C25" s="23" t="s">
+        <v>77</v>
+      </c>
+      <c r="D25" s="15" t="s">
         <v>78</v>
-      </c>
-      <c r="C25" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>80</v>
       </c>
       <c r="E25" s="12"/>
       <c r="F25" s="12"/>
@@ -1672,15 +1656,15 @@
       <c r="Y25" s="12"/>
       <c r="Z25" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="26" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="21" t="s">
+        <v>71</v>
+      </c>
+      <c r="C26" s="21" t="s">
         <v>72</v>
-      </c>
-      <c r="B26" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="C26" s="21" t="s">
-        <v>74</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="12"/>
@@ -1706,7 +1690,7 @@
       <c r="Y26" s="12"/>
       <c r="Z26" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="27" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="21"/>
       <c r="B27" s="21"/>
       <c r="C27" s="21"/>
@@ -1734,7 +1718,7 @@
       <c r="Y27" s="12"/>
       <c r="Z27" s="12"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="19.5" customFormat="1" s="7">
+    <row r="28" spans="1:26" s="7" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24"/>
       <c r="B28" s="24"/>
       <c r="C28" s="24"/>
@@ -1768,49 +1752,47 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:K17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1">
-      <pane state="frozen" activePane="bottomLeft" topLeftCell="A2" ySplit="1" xSplit="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="6" width="53.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="46.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="6" width="33.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="6" width="14.147857142857141" customWidth="1" bestFit="1"/>
+    <col min="1" max="2" width="53.7109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="46.85546875" style="6" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.5703125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="14.140625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
+    <row r="1" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1821,93 +1803,102 @@
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
+      <c r="K2" s="1"/>
+    </row>
+    <row r="3" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1"/>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
+      <c r="K3" s="1"/>
+    </row>
+    <row r="4" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
+      <c r="K4" s="1"/>
+    </row>
+    <row r="5" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
+      <c r="K5" s="1"/>
+    </row>
+    <row r="6" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="3"/>
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D7" s="5"/>
+      <c r="D7" s="3"/>
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="5"/>
+      <c r="K7" s="5"/>
+    </row>
+    <row r="8" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
       <c r="D8" s="5"/>
@@ -1917,81 +1908,91 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="19.5">
+      <c r="K8" s="5"/>
+    </row>
+    <row r="9" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="5"/>
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="19.5">
+      <c r="K9" s="5"/>
+    </row>
+    <row r="10" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="5"/>
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="19.5">
+      <c r="K10" s="5"/>
+    </row>
+    <row r="11" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="5"/>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="19.5">
+      <c r="K11" s="5"/>
+    </row>
+    <row r="12" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="5"/>
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5">
-      <c r="A13" s="5"/>
+      <c r="K12" s="5"/>
+    </row>
+    <row r="13" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
@@ -2001,64 +2002,72 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5">
+      <c r="K13" s="5"/>
+    </row>
+    <row r="14" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D14" s="5"/>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
+      <c r="K14" s="5"/>
+    </row>
+    <row r="15" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D15" s="5"/>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="19.5">
+      <c r="K15" s="5"/>
+    </row>
+    <row r="16" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D16" s="5"/>
+        <v>17</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5">
+      <c r="K16" s="5"/>
+    </row>
+    <row r="17" spans="1:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3"/>
-      <c r="B17" s="5"/>
+      <c r="B17" s="3"/>
       <c r="C17" s="5"/>
       <c r="D17" s="5"/>
       <c r="E17" s="5"/>
@@ -2067,6 +2076,7 @@
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
+      <c r="K17" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>